<commit_message>
Prototype risk analysis table complete, only two cells are active
</commit_message>
<xml_diff>
--- a/BACKEND/routes/data/riskAnalysis.xlsx
+++ b/BACKEND/routes/data/riskAnalysis.xlsx
@@ -323,47 +323,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -680,7 +640,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,16 +1229,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>